<commit_message>
changing the priority compare graph.
</commit_message>
<xml_diff>
--- a/Semantle_AI/Service/Reports_output/Noise_compare/Queue=True/Multi-Lateration/noise_effect_with_queue.xlsx
+++ b/Semantle_AI/Service/Reports_output/Noise_compare/Queue=True/Multi-Lateration/noise_effect_with_queue.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bardamri/SE_Project_Semantle/Semantle_AI/Service/Reports_output/Noise_compare/Queue=True/Multi-Lateration/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bardamri/PycharmProjects/SE_Project_Semantle/Semantle_AI/Service/Reports_output/Noise_compare/Queue=True/Multi-Lateration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02DC412-DF33-A847-AF40-07C6AE5BAA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA62405-C4A9-C44A-BF46-01F79D10C25A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17120" xr2:uid="{06FFA078-D96E-CA4E-BE05-FA592FBE15F9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{06FFA078-D96E-CA4E-BE05-FA592FBE15F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -204,6 +204,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -272,12 +275,24 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -313,18 +328,6 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
       <font>
@@ -480,7 +483,7 @@
             <c:numRef>
               <c:f>Sheet1!$N$3:$N$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
@@ -604,7 +607,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -810,7 +813,7 @@
             <c:numRef>
               <c:f>Sheet1!$O$3:$O$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -934,7 +937,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3038,8 +3041,8 @@
     <tableColumn id="3" xr3:uid="{676F4498-FEF3-EA47-B70A-D0F6DD060195}" name="5%"/>
     <tableColumn id="7" xr3:uid="{10D4614B-05E7-0C4B-9212-158119227CB5}" name="6%"/>
     <tableColumn id="8" xr3:uid="{C9A96573-5A53-834B-95BB-3A68EF910423}" name="7%" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{6E353E5C-4E64-5048-BF39-5399194671B9}" name="8%" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{FF27217B-4404-944A-90F8-E8053017F2FE}" name="9%" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{6E353E5C-4E64-5048-BF39-5399194671B9}" name="8%" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{FF27217B-4404-944A-90F8-E8053017F2FE}" name="9%" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{9E7E4807-0CB2-1C42-B388-2C936A0FDF52}" name="10%"/>
     <tableColumn id="5" xr3:uid="{81435C9D-3729-604E-A6CA-9983EDA9A677}" name="20%"/>
     <tableColumn id="6" xr3:uid="{EEB49D68-BC36-204D-AD38-A60D5AED05D3}" name="50%"/>
@@ -3052,16 +3055,16 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F340024C-3088-1F4C-BDDA-60C87C84B458}" name="Table4" displayName="Table4" ref="M2:P11" totalsRowShown="0">
   <autoFilter ref="M2:P11" xr:uid="{F340024C-3088-1F4C-BDDA-60C87C84B458}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{F5EB59AE-E081-E748-B720-29D23C2AAB66}" name="Noise" dataDxfId="5">
+    <tableColumn id="1" xr3:uid="{F5EB59AE-E081-E748-B720-29D23C2AAB66}" name="Noise" dataDxfId="3">
       <calculatedColumnFormula>Table3[[#Headers],[5%]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{B846D4F2-C4CB-274F-AB78-227097F7609A}" name="Average" dataDxfId="4">
+    <tableColumn id="2" xr3:uid="{B846D4F2-C4CB-274F-AB78-227097F7609A}" name="Average" dataDxfId="2">
       <calculatedColumnFormula>AVERAGE(C2:C41)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E26AF110-F15E-954D-A8C1-0E36D03DBA0F}" name="Variance" dataDxfId="3">
+    <tableColumn id="3" xr3:uid="{E26AF110-F15E-954D-A8C1-0E36D03DBA0F}" name="Variance" dataDxfId="0">
       <calculatedColumnFormula>VAR(B3:B42)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{D37321B9-DB97-E741-9239-14B0E37BD0D3}" name="Median" dataDxfId="2">
+    <tableColumn id="4" xr3:uid="{D37321B9-DB97-E741-9239-14B0E37BD0D3}" name="Median" dataDxfId="1">
       <calculatedColumnFormula>MEDIAN(C3:C42)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3369,7 +3372,7 @@
   <dimension ref="A1:P42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13:G22"/>
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3470,11 +3473,11 @@
         <f>B2</f>
         <v>0%</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="7">
         <f>AVERAGE(B3:B42)</f>
         <v>2</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="7">
         <f t="shared" ref="O3" si="0">VAR(B3:B42)</f>
         <v>0</v>
       </c>
@@ -3518,11 +3521,11 @@
         <f>C2</f>
         <v>5%</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="7">
         <f>AVERAGE(C3:C42)</f>
         <v>18.25</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="7">
         <f>VAR(C3:C42)</f>
         <v>206.55128205128204</v>
       </c>
@@ -3566,11 +3569,11 @@
         <f>D2</f>
         <v>6%</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="7">
         <f>AVERAGE(D3:D42)</f>
         <v>100.8</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="7">
         <f>VAR(D3:D42)</f>
         <v>69005.702564102568</v>
       </c>
@@ -3614,11 +3617,11 @@
         <f>E2</f>
         <v>7%</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="7">
         <f>AVERAGE(E3:E42)</f>
         <v>330</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="7">
         <f>VAR(E3:E42)</f>
         <v>293813.12820512819</v>
       </c>
@@ -3670,7 +3673,7 @@
         <f>VAR(F3:F42)</f>
         <v>599541.07628205128</v>
       </c>
-      <c r="P7" s="7">
+      <c r="P7">
         <f>MEDIAN(F3:F42)</f>
         <v>35.5</v>
       </c>
@@ -3718,7 +3721,7 @@
         <f>VAR(G3:G42)</f>
         <v>898133.4608974359</v>
       </c>
-      <c r="P8" s="7">
+      <c r="P8">
         <f>MEDIAN(G3:G42)</f>
         <v>585</v>
       </c>
@@ -3766,7 +3769,7 @@
         <f>VAR(H3:H42)</f>
         <v>1061270.8615384616</v>
       </c>
-      <c r="P9" s="7">
+      <c r="P9">
         <f>MEDIAN(H3:H42)</f>
         <v>1148.5</v>
       </c>
@@ -3806,11 +3809,11 @@
         <f>I2</f>
         <v>20%</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="7">
         <f>AVERAGE(I3:I42)</f>
         <v>2057.7249999999999</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="7">
         <f>VAR(I3:I42)</f>
         <v>1464368.4096153844</v>
       </c>
@@ -3854,11 +3857,11 @@
         <f>J2</f>
         <v>50%</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="7">
         <f>AVERAGE(J3:J42)</f>
         <v>2155.6</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="7">
         <f>VAR(J3:J42)</f>
         <v>1484380.6564102562</v>
       </c>

</xml_diff>